<commit_message>
Lots of changes. Fixed labeling for display/non-display groups to be correct. Added code for running a bunch of seeds. Added more outcome clusters (sepsis vs nonsepsis) (clinsepsis vs everything else). Added in code to calculate prior culture rate in window before culture.
</commit_message>
<xml_diff>
--- a/ModelComparisonv2.xlsx
+++ b/ModelComparisonv2.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="7 Day Mortality" sheetId="1" r:id="rId1"/>
     <sheet name="30 Day Mortality" sheetId="2" r:id="rId2"/>
+    <sheet name="7 Day Mortality Mean" sheetId="5" r:id="rId3"/>
+    <sheet name="30 Day Mortality Mean" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="59">
   <si>
     <t>30 Day Mortality</t>
   </si>
@@ -208,6 +210,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,11 +297,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,6 +306,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,28 +610,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
@@ -880,19 +895,19 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>981.6</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1054.5</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>0.74</v>
       </c>
       <c r="G14">
@@ -1156,19 +1171,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>13</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>973</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>1052</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0.75</v>
       </c>
       <c r="G26">
@@ -1294,19 +1309,19 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>6</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>969.3</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>1005.8</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>0.72</v>
       </c>
       <c r="G32">
@@ -1432,19 +1447,19 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>12</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>976</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>1048.9000000000001</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>0.73</v>
       </c>
       <c r="G38">
@@ -1570,19 +1585,19 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>7</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>960</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <v>1002.5</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>0.75</v>
       </c>
       <c r="G44">
@@ -1708,19 +1723,19 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>13</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>968</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>1047</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>0.75</v>
       </c>
       <c r="G50">
@@ -1836,7 +1851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -1846,28 +1861,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
@@ -2131,19 +2146,19 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1752.4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1825.3</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>0.77</v>
       </c>
       <c r="G14">
@@ -2407,19 +2422,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>13</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>1740.4</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>1819.3</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0.77</v>
       </c>
       <c r="G26">
@@ -2545,19 +2560,19 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>6</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>1759.8</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>1796.3</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>0.73</v>
       </c>
       <c r="G32">
@@ -2683,19 +2698,19 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>12</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>1751.8</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>1824.6</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>0.76</v>
       </c>
       <c r="G38">
@@ -2821,19 +2836,19 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>7</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>1742.7</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <v>1785.2</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>0.76</v>
       </c>
       <c r="G44">
@@ -2959,19 +2974,19 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>13</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>1741.6</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>1820.6</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>0.77</v>
       </c>
       <c r="G50">
@@ -3025,6 +3040,1896 @@
       </c>
       <c r="H52">
         <v>7.7780000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:B52">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C52">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D52">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>964.20131143808703</v>
+      </c>
+      <c r="D3" s="7">
+        <v>970.44406778380005</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.64135292524377097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>929.346997009289</v>
+      </c>
+      <c r="D4" s="7">
+        <v>941.83250970071799</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.68682803910356705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <v>914.40813532394804</v>
+      </c>
+      <c r="D5" s="7">
+        <v>933.13640436109097</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.70454306859676596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>908.86982665228004</v>
+      </c>
+      <c r="D6" s="7">
+        <v>933.840852035137</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.71383157026202804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>906.46693806517203</v>
+      </c>
+      <c r="D7" s="7">
+        <v>937.68071979374395</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.72441712060109997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7">
+        <v>906.09927636257805</v>
+      </c>
+      <c r="D8" s="7">
+        <v>943.55581443686401</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.72913919234781899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>906.37226139861195</v>
+      </c>
+      <c r="D9" s="7">
+        <v>950.07155581861298</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.73119162804462201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <v>906.985397890836</v>
+      </c>
+      <c r="D10" s="7">
+        <v>956.92744865655197</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.73263628064684505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7">
+        <v>906.96532149408904</v>
+      </c>
+      <c r="D11" s="7">
+        <v>963.15012860551997</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.73555096605272696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7">
+        <v>906.98721354129395</v>
+      </c>
+      <c r="D12" s="7">
+        <v>969.41477699843904</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.73881661048914604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>907.15371892952999</v>
+      </c>
+      <c r="D13" s="7">
+        <v>975.824038732389</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.74173796697564298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8">
+        <v>907.57034255093504</v>
+      </c>
+      <c r="D14" s="8">
+        <v>982.48341869950798</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.744220373881466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>924.76826025827802</v>
+      </c>
+      <c r="D15" s="7">
+        <v>937.25377294970804</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.70856907828739701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <v>916.759997326762</v>
+      </c>
+      <c r="D16" s="7">
+        <v>935.48826636390504</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.71367501304122505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7">
+        <v>908.60445485715604</v>
+      </c>
+      <c r="D17" s="7">
+        <v>933.57548024001403</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.72241558324306798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>906.11418759440005</v>
+      </c>
+      <c r="D18" s="7">
+        <v>937.32796932297299</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.72722001524820301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="7">
+        <v>905.23188116918095</v>
+      </c>
+      <c r="D19" s="7">
+        <v>942.68841924346805</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.73358833915174004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>905.39765065855397</v>
+      </c>
+      <c r="D20" s="7">
+        <v>949.096945078555</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.736926236908651</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7">
+        <v>905.93556179842199</v>
+      </c>
+      <c r="D21" s="7">
+        <v>955.87761256413796</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.73849261165284197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7">
+        <v>906.64345628035005</v>
+      </c>
+      <c r="D22" s="7">
+        <v>962.82826339178098</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.73987161931706102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23" s="7">
+        <v>906.97478018876302</v>
+      </c>
+      <c r="D23" s="7">
+        <v>969.40234364590697</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.74186987129330495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" s="7">
+        <v>907.08608365735302</v>
+      </c>
+      <c r="D24" s="7">
+        <v>975.75640346021305</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.74482868364032095</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25" s="7">
+        <v>907.44248460678295</v>
+      </c>
+      <c r="D25" s="7">
+        <v>982.35556075535703</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.74719894867783998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8">
+        <v>908.01386322971405</v>
+      </c>
+      <c r="D26" s="8">
+        <v>989.16969572400205</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.74921815436782002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>932.22253098366002</v>
+      </c>
+      <c r="D27" s="7">
+        <v>938.46528732937202</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.66547030278600405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>896.24250924895102</v>
+      </c>
+      <c r="D28" s="7">
+        <v>908.72802194038104</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.7060971664522</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <v>881.22551005019</v>
+      </c>
+      <c r="D29" s="7">
+        <v>899.95377908733406</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.72250512911944498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7">
+        <v>875.35358549413195</v>
+      </c>
+      <c r="D30" s="7">
+        <v>900.32461087699005</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.73453907691353604</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" s="7">
+        <v>871.77392893232798</v>
+      </c>
+      <c r="D31" s="7">
+        <v>902.98771066090103</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0.74467603861438803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="4">
+        <v>6</v>
+      </c>
+      <c r="C32" s="12">
+        <v>871.09683141048401</v>
+      </c>
+      <c r="D32" s="12">
+        <v>908.553369484771</v>
+      </c>
+      <c r="E32" s="15">
+        <v>0.74960464437243901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" s="7">
+        <v>871.35859523037698</v>
+      </c>
+      <c r="D33" s="7">
+        <v>915.057889650378</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0.75203880559991299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
+        <v>872.00750773421305</v>
+      </c>
+      <c r="D34" s="7">
+        <v>921.94955849992903</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.75378452788845696</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7">
+        <v>871.86894054068102</v>
+      </c>
+      <c r="D35" s="7">
+        <v>928.05374765211195</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0.75658156462690496</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36" s="7">
+        <v>871.78579847738695</v>
+      </c>
+      <c r="D36" s="7">
+        <v>934.21336193453203</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0.75993638341524405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37" s="7">
+        <v>871.87812276531599</v>
+      </c>
+      <c r="D37" s="7">
+        <v>940.54844256817603</v>
+      </c>
+      <c r="E37" s="13">
+        <v>0.76272292936026898</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2">
+        <v>12</v>
+      </c>
+      <c r="C38" s="8">
+        <v>872.18185632519203</v>
+      </c>
+      <c r="D38" s="8">
+        <v>947.09493247376497</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.765255616191997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>892.00707170236205</v>
+      </c>
+      <c r="D39" s="7">
+        <v>904.49258439379105</v>
+      </c>
+      <c r="E39" s="13">
+        <v>0.73514364118384801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7">
+        <v>884.00986681092797</v>
+      </c>
+      <c r="D40" s="7">
+        <v>902.73813584807203</v>
+      </c>
+      <c r="E40" s="13">
+        <v>0.73964616827645102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="7">
+        <v>875.96471529566304</v>
+      </c>
+      <c r="D41" s="7">
+        <v>900.93574067852001</v>
+      </c>
+      <c r="E41" s="13">
+        <v>0.74812026170136203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" s="7">
+        <v>873.15744282574406</v>
+      </c>
+      <c r="D42" s="7">
+        <v>904.37122455431597</v>
+      </c>
+      <c r="E42" s="13">
+        <v>0.75378268037187501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" s="7">
+        <v>871.23451524906</v>
+      </c>
+      <c r="D43" s="7">
+        <v>908.69105332334698</v>
+      </c>
+      <c r="E43" s="13">
+        <v>0.75791233210854303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="4">
+        <v>7</v>
+      </c>
+      <c r="C44" s="12">
+        <v>871.04418203193802</v>
+      </c>
+      <c r="D44" s="12">
+        <v>914.74347645193905</v>
+      </c>
+      <c r="E44" s="15">
+        <v>0.76092930083771204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45" s="7">
+        <v>871.55240600875402</v>
+      </c>
+      <c r="D45" s="7">
+        <v>921.49445677446897</v>
+      </c>
+      <c r="E45" s="13">
+        <v>0.76264917081388806</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46" s="7">
+        <v>872.27619765342797</v>
+      </c>
+      <c r="D46" s="7">
+        <v>928.46100476485799</v>
+      </c>
+      <c r="E46" s="13">
+        <v>0.76431763331834501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47" s="7">
+        <v>872.46766513202294</v>
+      </c>
+      <c r="D47" s="7">
+        <v>934.895228589167</v>
+      </c>
+      <c r="E47" s="13">
+        <v>0.76609228280698405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48" s="7">
+        <v>872.47764609748003</v>
+      </c>
+      <c r="D48" s="7">
+        <v>941.14796590033905</v>
+      </c>
+      <c r="E48" s="13">
+        <v>0.76877534198436204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49" s="7">
+        <v>872.76091661602504</v>
+      </c>
+      <c r="D49" s="7">
+        <v>947.67399276459798</v>
+      </c>
+      <c r="E49" s="13">
+        <v>0.77073188787770697</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2">
+        <v>13</v>
+      </c>
+      <c r="C50" s="8">
+        <v>873.20123998545398</v>
+      </c>
+      <c r="D50" s="8">
+        <v>954.35707247974199</v>
+      </c>
+      <c r="E50" s="14">
+        <v>0.772482390453895</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>932.85362922310105</v>
+      </c>
+      <c r="D51" s="7">
+        <v>939.09638556881703</v>
+      </c>
+      <c r="E51" s="13">
+        <v>0.70817658801813499</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" s="7">
+        <v>910.25043312109801</v>
+      </c>
+      <c r="D52" s="7">
+        <v>947.70697119538499</v>
+      </c>
+      <c r="E52" s="13">
+        <v>0.74152735143053505</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:B52">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C52">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D52">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E52">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1760.03351847668</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1766.27627482239</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.64416944042408697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1684.70363653599</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1697.1891492274201</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.70141768795315795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1666.8682897823801</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1685.5965588195199</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.71180441163370001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1661.8778921450901</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1686.8489175279501</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.716357347882978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1658.3238659293399</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1689.5376476579199</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.72142699551455403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1657.5934884630799</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1695.0500265373601</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.72370450199051095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1658.0442234280699</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1701.74351784808</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.72440432185535697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1658.67725750256</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1708.6193082682801</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.72490273048796205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1658.7422647339299</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1714.9270718453599</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.72621232577968897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1658.5669434731899</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1720.9945069303401</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.72781368333003604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1658.64735438516</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1727.31767418802</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.72924188784417499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1658.5960030383001</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1733.5090791868699</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.73086729233841397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1683.5095327768299</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1695.9950454682601</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.70508971471080795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1663.1087407478401</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1681.83700978498</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.71857567701084701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1655.9500648753699</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1680.9210902582199</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.72289817446847704</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1654.6425355962399</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1685.8563173248101</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.72480595845900797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1653.5229644347501</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1690.97950250904</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.72722575666598599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1653.87917814107</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1697.5784725610699</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.72847487883973305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1654.6231194069101</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1704.5651701726199</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.729016580069905</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1655.43547239996</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1711.62027951139</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.72948202755593905</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1655.9755492573599</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1718.4031127144999</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.73037948125241203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1655.9964795217199</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1724.6667993245701</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.73171463329134201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1656.3947280934101</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1731.30780424199</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.73270835574900095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1656.5455964380899</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1737.7014289323799</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.73403655459414596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1720.60078188941</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1726.8435382351199</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.62307609321058599</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1641.1026239651401</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1653.58813665657</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.69181564657652495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1621.67105686734</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1640.3993259044901</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.70981245205216703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1616.00664607676</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1640.9776714596201</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.71651469001726098</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1611.5014710148</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1642.71525274338</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0.72326742903720798</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="4">
+        <v>6</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1610.4840566768801</v>
+      </c>
+      <c r="D32" s="12">
+        <v>1647.94059475117</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0.726075895425776</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1610.97567944547</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1654.6749738654701</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0.72725590957038799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1611.63905772054</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1661.5811084862601</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0.72807665060414295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1611.60702007897</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1667.7918271904</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0.72962486814345995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1611.3992875822801</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1673.82685103942</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0.73134069931914103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1611.4492833898</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1680.11960319266</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0.73293596566935204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2">
+        <v>12</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1611.3847764541399</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1686.29785260271</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0.73464546173762901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1637.6218060747899</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1650.10731876621</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0.71359740602224997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1617.1472596127601</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1635.8755286498999</v>
+      </c>
+      <c r="E40" s="9">
+        <v>0.72562049290372199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1609.53574304156</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1634.50676842442</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0.73013421197737305</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1607.97240837046</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1639.18619009903</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0.73163888689106804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1606.34097237993</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1643.7975104542199</v>
+      </c>
+      <c r="E43" s="9">
+        <v>0.73369261243767603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="4">
+        <v>7</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1606.5162895414801</v>
+      </c>
+      <c r="D44" s="12">
+        <v>1650.21558396148</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0.73489000167818197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45" s="7">
+        <v>1607.3699612458699</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1657.31201201158</v>
+      </c>
+      <c r="E45" s="9">
+        <v>0.7356375023974</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1608.2517768893999</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1664.43658400083</v>
+      </c>
+      <c r="E46" s="9">
+        <v>0.73628657220944405</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1608.77714904408</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1671.20471250122</v>
+      </c>
+      <c r="E47" s="9">
+        <v>0.73722288550058301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1608.8167400265299</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1677.4870598293901</v>
+      </c>
+      <c r="E48" s="9">
+        <v>0.73840625000000704</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49" s="7">
+        <v>1609.2564803903499</v>
+      </c>
+      <c r="D49" s="7">
+        <v>1684.16955653893</v>
+      </c>
+      <c r="E49" s="9">
+        <v>0.73931382455888695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2">
+        <v>13</v>
+      </c>
+      <c r="C50" s="8">
+        <v>1609.4282655243101</v>
+      </c>
+      <c r="D50" s="8">
+        <v>1690.5840980185999</v>
+      </c>
+      <c r="E50" s="10">
+        <v>0.740498471662838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>1708.8013606214899</v>
+      </c>
+      <c r="D51" s="7">
+        <v>1715.0441169671999</v>
+      </c>
+      <c r="E51" s="9">
+        <v>0.69012183707776298</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1671.1007433105001</v>
+      </c>
+      <c r="D52" s="7">
+        <v>1708.55728138478</v>
+      </c>
+      <c r="E52" s="9">
+        <v>0.72052560244623598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>